<commit_message>
Hà cập nhật tính năng, fix bugs 🐷🐷🐷
</commit_message>
<xml_diff>
--- a/danhsachsinhvien.xlsx
+++ b/danhsachsinhvien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam3_Ki_II\LapTrinhMang\quan-ly-phong-thi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\quan-ly-phong-thi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD78DDBA-AB6A-43B9-9712-B3B119DFDC6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA60FDF-9EB9-4072-8377-2259E942662F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{B48D1D37-B239-4BDE-A3E3-CD7B8B693963}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B48D1D37-B239-4BDE-A3E3-CD7B8B693963}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="150">
   <si>
     <t>MSSV</t>
   </si>
@@ -54,19 +54,454 @@
   </si>
   <si>
     <t>Hiếu</t>
+  </si>
+  <si>
+    <t>Hoàng Ngọc</t>
+  </si>
+  <si>
+    <t>Anh</t>
+  </si>
+  <si>
+    <t>Nguyễn Trần Việt</t>
+  </si>
+  <si>
+    <t>Vũ Tuấn</t>
+  </si>
+  <si>
+    <t>Bùi Quốc</t>
+  </si>
+  <si>
+    <t>Bảo</t>
+  </si>
+  <si>
+    <t>Phan Lê Quốc</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh</t>
+  </si>
+  <si>
+    <t>Cường</t>
+  </si>
+  <si>
+    <t>Nguyễn</t>
+  </si>
+  <si>
+    <t>Danh</t>
+  </si>
+  <si>
+    <t>Phạm Trung Anh</t>
+  </si>
+  <si>
+    <t>Dũng</t>
+  </si>
+  <si>
+    <t>Võ Thành</t>
+  </si>
+  <si>
+    <t>Duy</t>
+  </si>
+  <si>
+    <t>Trần Nguyễn Đông</t>
+  </si>
+  <si>
+    <t>Gon</t>
+  </si>
+  <si>
+    <t>Lê Quốc</t>
+  </si>
+  <si>
+    <t>Hoàng</t>
+  </si>
+  <si>
+    <t>Lê Sỹ</t>
+  </si>
+  <si>
+    <t>Hùng</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn</t>
+  </si>
+  <si>
+    <t>Hà Nguyễn Đức</t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>Hà Quốc</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Việt</t>
+  </si>
+  <si>
+    <t>Phạm</t>
+  </si>
+  <si>
+    <t>Nguyễn Quốc</t>
+  </si>
+  <si>
+    <t>Hưng</t>
+  </si>
+  <si>
+    <t>Khánh</t>
+  </si>
+  <si>
+    <t>Lê Anh</t>
+  </si>
+  <si>
+    <t>Khoa</t>
+  </si>
+  <si>
+    <t>Nguyễn Lê Đăng</t>
+  </si>
+  <si>
+    <t>Lê Phạm Minh</t>
+  </si>
+  <si>
+    <t>Khôi</t>
+  </si>
+  <si>
+    <t>Nguyễn Trung</t>
+  </si>
+  <si>
+    <t>Kiên</t>
+  </si>
+  <si>
+    <t>Vũ Hoàng</t>
+  </si>
+  <si>
+    <t>Lâm</t>
+  </si>
+  <si>
+    <t>Nguyễn Khánh</t>
+  </si>
+  <si>
+    <t>Linh</t>
+  </si>
+  <si>
+    <t>Lê Văn</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Nguyễn Bảo</t>
+  </si>
+  <si>
+    <t>Phan Trương Ngọc</t>
+  </si>
+  <si>
+    <t>Trần Vũ</t>
+  </si>
+  <si>
+    <t>Lộc</t>
+  </si>
+  <si>
+    <t>Nguyễn Thành</t>
+  </si>
+  <si>
+    <t>Luân</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Nguyễn Hữu Nhật</t>
+  </si>
+  <si>
+    <t>Minh</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Diễm</t>
+  </si>
+  <si>
+    <t>My</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Quỳnh</t>
+  </si>
+  <si>
+    <t>Nga</t>
+  </si>
+  <si>
+    <t>Nghiệm</t>
+  </si>
+  <si>
+    <t>Nguyễn Bình Phương</t>
+  </si>
+  <si>
+    <t>Nguyên</t>
+  </si>
+  <si>
+    <t>Trần Hoàng Trung</t>
+  </si>
+  <si>
+    <t>Phan Công Trọng</t>
+  </si>
+  <si>
+    <t>Nhân</t>
+  </si>
+  <si>
+    <t>Lê Hoàng</t>
+  </si>
+  <si>
+    <t>Nhật</t>
+  </si>
+  <si>
+    <t>Hoàng Thị Hồng</t>
+  </si>
+  <si>
+    <t>Nhung</t>
+  </si>
+  <si>
+    <t>Trịnh Nguyễn Hồng</t>
+  </si>
+  <si>
+    <t>Phi</t>
+  </si>
+  <si>
+    <t>Tạ Cao</t>
+  </si>
+  <si>
+    <t>Phong</t>
+  </si>
+  <si>
+    <t>Chương Xuân Hoàng</t>
+  </si>
+  <si>
+    <t>Phúc</t>
+  </si>
+  <si>
+    <t>Vi Văn</t>
+  </si>
+  <si>
+    <t>Vũ Đình</t>
+  </si>
+  <si>
+    <t>Hoàng Minh</t>
+  </si>
+  <si>
+    <t>Phương</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Bảo</t>
+  </si>
+  <si>
+    <t>Võ Thị Thuý</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồng</t>
+  </si>
+  <si>
+    <t>Phượng</t>
+  </si>
+  <si>
+    <t>Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Quang</t>
+  </si>
+  <si>
+    <t>Hoàng Vinh</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc</t>
+  </si>
+  <si>
+    <t>Trần Hữu Khải</t>
+  </si>
+  <si>
+    <t>Quân</t>
+  </si>
+  <si>
+    <t>Phạm Lê Anh</t>
+  </si>
+  <si>
+    <t>Quốc</t>
+  </si>
+  <si>
+    <t>Cao Hoàng</t>
+  </si>
+  <si>
+    <t>Sang</t>
+  </si>
+  <si>
+    <t>Đinh Bá Thái</t>
+  </si>
+  <si>
+    <t>Sơn</t>
+  </si>
+  <si>
+    <t>Đỗ Trường</t>
+  </si>
+  <si>
+    <t>Huỳnh Chí</t>
+  </si>
+  <si>
+    <t>Tài</t>
+  </si>
+  <si>
+    <t>Phạm Văn</t>
+  </si>
+  <si>
+    <t>Tâm</t>
+  </si>
+  <si>
+    <t>Huỳnh Thiên</t>
+  </si>
+  <si>
+    <t>Tân</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Cảnh</t>
+  </si>
+  <si>
+    <t>Đặng Ngọc</t>
+  </si>
+  <si>
+    <t>Thạch</t>
+  </si>
+  <si>
+    <t>Văn Hữu</t>
+  </si>
+  <si>
+    <t>Thành</t>
+  </si>
+  <si>
+    <t>Tôn Thất</t>
+  </si>
+  <si>
+    <t>Thắng</t>
+  </si>
+  <si>
+    <t>Hồ Ngọc Bảo</t>
+  </si>
+  <si>
+    <t>Thiên</t>
+  </si>
+  <si>
+    <t>Ngô Văn</t>
+  </si>
+  <si>
+    <t>Thịnh</t>
+  </si>
+  <si>
+    <t>Triệu Tiến</t>
+  </si>
+  <si>
+    <t>Phạm Trần Phúc</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Phương</t>
+  </si>
+  <si>
+    <t>Thủy</t>
+  </si>
+  <si>
+    <t>Toàn</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Thùy</t>
+  </si>
+  <si>
+    <t>Trang</t>
+  </si>
+  <si>
+    <t>Nguyễn Đình Phát</t>
+  </si>
+  <si>
+    <t>Triển</t>
+  </si>
+  <si>
+    <t>Đặng Thành</t>
+  </si>
+  <si>
+    <t>Trung</t>
+  </si>
+  <si>
+    <t>Huỳnh Văn</t>
+  </si>
+  <si>
+    <t>Nguyễn Mậu</t>
+  </si>
+  <si>
+    <t>Tuấn</t>
+  </si>
+  <si>
+    <t>Phạm Minh</t>
+  </si>
+  <si>
+    <t>Trần Văn</t>
+  </si>
+  <si>
+    <t>Tứ</t>
+  </si>
+  <si>
+    <t>Dương Văn</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Hồng</t>
+  </si>
+  <si>
+    <t>Vân</t>
+  </si>
+  <si>
+    <t>Lưu Đỗ Hoàng</t>
+  </si>
+  <si>
+    <t>Viễn</t>
+  </si>
+  <si>
+    <t>Trương Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Việt</t>
+  </si>
+  <si>
+    <t>Bùi Thanh Tuyến</t>
+  </si>
+  <si>
+    <t>Nguyễn Đặng Quang</t>
+  </si>
+  <si>
+    <t>Vinh</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng</t>
+  </si>
+  <si>
+    <t>Vũ</t>
+  </si>
+  <si>
+    <t>Phan Quang</t>
+  </si>
+  <si>
+    <t>Lê Ngô Đăng</t>
+  </si>
+  <si>
+    <t>Vương</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,7 +512,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -85,12 +520,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,18 +912,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191C8A50-BFA7-465F-8DEC-7BF2CFCA1B6B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="A4:E6"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,29 +934,1020 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1812725</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1812726</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>1812727</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>1812728</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>1812731</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>1812733</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1812736</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>1812745</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>1812747</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>1812749</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>1812751</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>1812756</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C13" s="4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>1812759</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>1812767</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>1812768</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>1812770</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>1812771</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>1812772</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>1812774</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>1812769</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>1812779</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>1812780</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>1812781</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>1812783</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>1812785</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>1812788</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>1812790</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>1812794</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>1812795</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>1812798</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>1812793</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>1812800</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>1813758</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>1812801</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>1812802</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>1812803</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>1812805</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>1812807</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>1812808</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>1812809</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>1812813</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>1812814</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>1812816</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>1812818</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>1812819</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>1812821</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>1812823</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>1812824</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>1812825</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>1812826</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>1812828</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>1812829</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>1812830</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>1812831</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
+        <v>1812832</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
+        <v>1813857</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="3">
+        <v>1812833</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
+        <v>1812834</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
+        <v>1812835</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
+        <v>1812836</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
+        <v>1812838</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
+        <v>1812840</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <v>1812841</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
+        <v>1812842</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
+        <v>1812843</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>1812847</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <v>1812844</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="3">
+        <v>1813809</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3">
+        <v>1812850</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3">
+        <v>1812851</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3">
+        <v>1813772</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3">
+        <v>1812853</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3">
+        <v>1812856</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="3">
+        <v>1812858</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
+        <v>1812859</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="3">
+        <v>1812860</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="3">
+        <v>1812863</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3">
+        <v>1812864</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>1812866</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
+        <v>1812867</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3">
+        <v>1812865</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <v>1813766</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>1812873</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>1812876</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <v>1812877</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
+        <v>1813808</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <v>1812878</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3">
+        <v>1812880</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="3">
+        <v>1812881</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="3">
+        <v>1812882</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="3">
+        <v>1812879</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="3">
+        <v>1813865</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>